<commit_message>
Add Affects Star Test
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test9_InterProcedural/ExcelQuery.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test9_InterProcedural/ExcelQuery.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="756" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="650" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uses" sheetId="15" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="221">
   <si>
     <t>Index</t>
   </si>
@@ -467,6 +467,228 @@
   </si>
   <si>
     <t>56</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(52, 53)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(36, 37)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(15, 16)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(100, 100)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(56, 56)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(72,72)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(50, 52)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(100, 103)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(104,107)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(107, 111)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(69, 71)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(39, 41)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(82, 85)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(107, 109)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(89, 94)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(65, 57)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(82, 88)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(43, 44)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(83,85)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(44, 45)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(82, _)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(_, 94)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(_, _)</t>
+  </si>
+  <si>
+    <t>Select s such that Affects*(82, s)</t>
+  </si>
+  <si>
+    <t>Select w such that Affects*(82, w)</t>
+  </si>
+  <si>
+    <t>Select f such that Affects*(43, f)</t>
+  </si>
+  <si>
+    <t>Select cl such that Affects*(51, 54)</t>
+  </si>
+  <si>
+    <t>Select v such that Affects*(59, v)</t>
+  </si>
+  <si>
+    <t>Select c such that Affects*(65, c)</t>
+  </si>
+  <si>
+    <t>Select s such that Affects*(_, s)</t>
+  </si>
+  <si>
+    <t>Select a such that Affects*(_, a)</t>
+  </si>
+  <si>
+    <t>Select pl such that Affects*(_, pl)</t>
+  </si>
+  <si>
+    <t>Select w such that Affects*(_, w)</t>
+  </si>
+  <si>
+    <t>Select f such that Affects*(_, f)</t>
+  </si>
+  <si>
+    <t>Select cl such that Affects*(_, cl)</t>
+  </si>
+  <si>
+    <t>Select p such that Affects*(_, p)</t>
+  </si>
+  <si>
+    <t>Select v such that Affects*(_, v)</t>
+  </si>
+  <si>
+    <t>Select c such that Affects*(_, c)</t>
+  </si>
+  <si>
+    <t>Select s1 such that Affects*(s1, s2)</t>
+  </si>
+  <si>
+    <t>Select s such that Affects*(s, a)</t>
+  </si>
+  <si>
+    <t>Select a such that Affects*(a, s)</t>
+  </si>
+  <si>
+    <t>Select a1 such that Affects*(a1, a2)</t>
+  </si>
+  <si>
+    <t>Select s1 such that Affects*(s1, s2) and Affects*(a1,a2)</t>
+  </si>
+  <si>
+    <t>Select s1 such that Affects*(s1, s2) and Affects*(s1, s3)</t>
+  </si>
+  <si>
+    <t>Select s1 such that Affects*(s1, s2) and Affects*(s1, a)</t>
+  </si>
+  <si>
+    <t>Select a1 such that Affects*(a1, a2) and Affects*(a1,a3)</t>
+  </si>
+  <si>
+    <t>Select a1 such that Affects*(a1, a2) and Affects*(a1, s)</t>
+  </si>
+  <si>
+    <t>Select s2 such that Affects*(s1, s2) and Affects*(s3, s2)</t>
+  </si>
+  <si>
+    <t>Select s2 such that Affects*(s1, s2) and Affects*(a, s2)</t>
+  </si>
+  <si>
+    <t>Select a2 such that Affects*(a1, a2) and Affects*(a3,a2)</t>
+  </si>
+  <si>
+    <t>Select a2 such that Affects*(a1, a2) and Affects*(s, a2)</t>
+  </si>
+  <si>
+    <t>Select s2 such that Affects*(s1, s2) and Affects*(s2, s3)</t>
+  </si>
+  <si>
+    <t>Select s2 such that Affects*(s1, s2) and Affects*(s2, a)</t>
+  </si>
+  <si>
+    <t>Select a such that Affects*(s1, a) and Affects*(a, s2)</t>
+  </si>
+  <si>
+    <t>Select a2 such that Affects*(a1, a2) and Affects*(a2, a3)</t>
+  </si>
+  <si>
+    <t>Select a2 such that Affects*(a1, a2) and Affects*(a2, s)</t>
+  </si>
+  <si>
+    <t>Select s such that Affects*(a1, s) and Affects*(s, a2)</t>
+  </si>
+  <si>
+    <t>Select s2 such that Affects*(s1, s2) and Affects*(s2, s1)</t>
+  </si>
+  <si>
+    <t>Select s such that Affects*(a, s) and Affects*(s,a)</t>
+  </si>
+  <si>
+    <t>Select a2 such that Affects*(a1, a2) and Affects*(a2,a1)</t>
+  </si>
+  <si>
+    <t>Select a such that Affects*(s, a) and Affects*(a,s)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN such that Affects*(102, 104)</t>
+  </si>
+  <si>
+    <t>Select &lt;a1, a2&gt; such that Affects*(a1, a2)</t>
+  </si>
+  <si>
+    <t>Get all AffectsStar</t>
+  </si>
+  <si>
+    <t>Select a such that Affects*(97, a)</t>
+  </si>
+  <si>
+    <t>Select pl such that Affects*(50, pl)</t>
+  </si>
+  <si>
+    <t>Int ProgLine - Skip a line inbtwn</t>
+  </si>
+  <si>
+    <t>assign a1,a2;</t>
+  </si>
+  <si>
+    <t>85,86,89,92,94</t>
+  </si>
+  <si>
+    <t>100,101,102,103,106,107,109,110,111,98,99</t>
+  </si>
+  <si>
+    <t>51,52,53</t>
+  </si>
+  <si>
+    <t>Select pl such that Affects*(68, pl)</t>
+  </si>
+  <si>
+    <t>procedure pl;</t>
+  </si>
+  <si>
+    <t>100 101,100 103,100 106,100 107,100 109,100 111,101 103,101 106,101 107,101 109,101 111,102 103,102 106,102 109,102 110,103 106,103 109,104 107,104 109,104 110,104 111,107 109,107 111,12 13,2 4,50 51,50 52,50 53,51 53,56 56,60 61,69 71,69 72,69 73,69 74,71 72,71 73,71 74,72 73,72 74,73 74,75 76,77 80,81 82,81 85,81 86,81 89,81 92,81 94,82 85,82 86,82 89,82 92,82 94,85 89,85 94,89 94,91 94,91 96,97 100,97 101,97 102,97 103,97 106,97 107,97 109,97 110,97 111,97 98,97 99,98 100,98 101,98 102,98 103,98 106,98 107,98 109,98 110,98 111,98 99,99 102,99 103,99 106,99 109,99 110</t>
   </si>
 </sst>
 </file>
@@ -538,7 +760,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -560,6 +782,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1228,7 +1453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{194B82F5-39A8-4622-BFD4-D2AAB88D40FF}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -1312,19 +1537,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85EBA76E-2EF5-4A75-9254-B8F09F669B64}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="40.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="87.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="38" style="4" customWidth="1"/>
     <col min="6" max="6" width="47.28515625" style="4" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="4"/>
@@ -1351,6 +1576,1058 @@
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>21</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>23</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>24</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>25</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>31</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>32</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>33</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>34</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>35</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <v>36</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <v>37</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
+        <v>38</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
+        <v>39</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <v>40</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>41</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>42</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>43</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>44</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>45</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>46</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>47</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>48</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>49</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>50</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>51</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
+        <v>52</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>53</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>54</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="6">
+        <v>55</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
+        <v>56</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>57</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>58</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="6">
+        <v>59</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="6">
+        <v>60</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="6">
+        <v>61</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="6">
+        <v>62</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="6">
+        <v>63</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="6">
+        <v>64</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="6">
+        <v>65</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="6">
+        <v>66</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1371,16 +2648,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD5F34A-C32F-4F9E-A4EF-99404DBA2DE9}">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" style="4" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="5" customWidth="1"/>
     <col min="5" max="5" width="38" style="4" customWidth="1"/>
     <col min="6" max="6" width="47.28515625" style="4" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>

</xml_diff>

<commit_message>
Update Next tests for inte procedure
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test9_InterProcedural/ExcelQuery.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test9_InterProcedural/ExcelQuery.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uses" sheetId="15" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="464">
   <si>
     <t>Index</t>
   </si>
@@ -1133,6 +1133,291 @@
   </si>
   <si>
     <t>Aaron cancel,Aaron difficulty,Aaron easy,Aaron exam,Aaron exercise,Aaron happy,Aaron kindess,Aaron kindness,Aaron laugh,Aaron lecture,Aaron love,Aaron skip,Aaron stress,Aaron tired,Aaron tutorial,Ben cancel,Ben difficulty,Ben easy,Ben exam,Ben exercise,Ben happy,Ben kindess,Ben kindness,Ben laugh,Ben lecture,Ben love,Ben skip,Ben stress,Ben tired,Ben tutorial,Colin cancel,Colin difficulty,Colin easy,Colin exam,Colin exercise,Colin happy,Colin kindess,Colin kindness,Colin laugh,Colin lecture,Colin love,Colin skip,Colin stress,Colin tired,Colin tutorial,Cristina cancel,Cristina easy,Cristina exam,Cristina exercise,Cristina happy,Cristina kindess,Cristina kindness,Cristina laugh,Cristina lecture,Cristina love,Cristina skip,Cristina stress,Cristina tired,Cristina tutorial,Damith cancel,Damith difficulty,Damith easy,Damith exam,Damith exercise,Damith happy,Damith kindess,Damith kindness,Damith laugh,Damith lecture,Damith love,Damith skip,Damith stress,Damith tired,Damith tutorial,EeChien cancel,EeChien difficulty,EeChien easy,EeChien exam,EeChien exercise,EeChien happy,EeChien kindess,EeChien kindness,EeChien laugh,EeChien lecture,EeChien love,EeChien skip,EeChien stress,EeChien tired,EeChien tutorial,Gary cancel,Gary difficulty,Gary easy,Gary exam,Gary exercise,Gary happy,Gary kindess,Gary kindness,Gary laugh,Gary lecture,Gary love,Gary skip,Gary stress,Gary tired,Gary tutorial,Hugh cancel,Hugh easy,Hugh exam,Hugh exercise,Hugh happy,Hugh kindess,Hugh kindness,Hugh laugh,Hugh lecture,Hugh love,Hugh skip,Hugh stress,Hugh tired,Hugh tutorial,Ian cancel,Ian easy,Ian exam,Ian exercise,Ian happy,Ian kindess,Ian kindness,Ian laugh,Ian lecture,Ian love,Ian skip,Ian stress,Ian tired,Ian tutorial,Jin cancel,Jin easy,Jin exam,Jin exercise,Jin happy,Jin kindess,Jin kindness,Jin laugh,Jin lecture,Jin love,Jin skip,Jin stress,Jin tired,Jin tutorial,MinYen cancel,MinYen exam,MinYen happy,MinYen kindess,MinYen kindness,MinYen lecture,MinYen skip,MinYen stress,MinYen tutorial,Parvathy cancel,Parvathy easy,Parvathy exam,Parvathy exercise,Parvathy happy,Parvathy kindess,Parvathy kindness,Parvathy laugh,Parvathy lecture,Parvathy skip,Parvathy stress,Parvathy tired,Parvathy tutorial,RayYan exam,RayYan happy,RayYan kindness,RayYan tired,RayYan tutorial,Steven cancel,Steven difficulty,Steven easy,Steven exam,Steven exercise,Steven happy,Steven kindess,Steven kindness,Steven laugh,Steven lecture,Steven love,Steven skip,Steven stress,Steven tired,Steven tutorial,Thilina cancel,Thilina easy,Thilina exam,Thilina exercise,Thilina happy,Thilina kindess,Thilina kindness,Thilina laugh,Thilina lecture,Thilina skip,Thilina stress,Thilina tired,Thilina tutorial,UncleSoo cancel,UncleSoo exam,UncleSoo happy,UncleSoo kindess,UncleSoo kindness,UncleSoo lecture,UncleSoo skip,UncleSoo stress,UncleSoo tutorial,WeeSun cancel,WeeSun easy,WeeSun exam,WeeSun exercise,WeeSun happy,WeeSun kindess,WeeSun kindness,WeeSun laugh,WeeSun lecture,WeeSun love,WeeSun skip,WeeSun stress,WeeSun tired,WeeSun tutorial,Wynne cancel,Wynne happy,Wynne kindess,Wynne kindness,Wynne lecture,Wynne skip,Wynne stress,Wynne tutorial</t>
+  </si>
+  <si>
+    <t>stmt s1, s2;</t>
+  </si>
+  <si>
+    <t>Select &lt;s1, s2&gt; such that Next(s1, s2)</t>
+  </si>
+  <si>
+    <t>stmt s; while w;</t>
+  </si>
+  <si>
+    <t>stmt s; if f;</t>
+  </si>
+  <si>
+    <t>stmt s; prog_line pl;</t>
+  </si>
+  <si>
+    <t>stmt s; call cl;</t>
+  </si>
+  <si>
+    <t>assign a; stmt s;</t>
+  </si>
+  <si>
+    <t>assign a; while w;</t>
+  </si>
+  <si>
+    <t>assign a; if f;</t>
+  </si>
+  <si>
+    <t>assign a; call cl;</t>
+  </si>
+  <si>
+    <t>while w1, w2;</t>
+  </si>
+  <si>
+    <t>while w; stmt s;</t>
+  </si>
+  <si>
+    <t>while w; assign a;</t>
+  </si>
+  <si>
+    <t>while w; if f;</t>
+  </si>
+  <si>
+    <t>while w; call cl;</t>
+  </si>
+  <si>
+    <t>if f1, f2;</t>
+  </si>
+  <si>
+    <t>if f; stmt s;</t>
+  </si>
+  <si>
+    <t>if f; assign a;</t>
+  </si>
+  <si>
+    <t>if f; while w;</t>
+  </si>
+  <si>
+    <t>if f; call cl;</t>
+  </si>
+  <si>
+    <t>call cl1,cl2;</t>
+  </si>
+  <si>
+    <t>call cl; stmt s;</t>
+  </si>
+  <si>
+    <t>call cl; assign a;</t>
+  </si>
+  <si>
+    <t>call cl; while w;</t>
+  </si>
+  <si>
+    <t>call cl; if f;</t>
+  </si>
+  <si>
+    <t>Select &lt;s, a&gt; such that Next(s, a)</t>
+  </si>
+  <si>
+    <t>Select &lt;s, w&gt; such that Next(s, w)</t>
+  </si>
+  <si>
+    <t>Select &lt;a, s&gt; such that Next(a, s)</t>
+  </si>
+  <si>
+    <t>Select &lt;a, w&gt; such that Next(a, w)</t>
+  </si>
+  <si>
+    <t>Select &lt;w, s&gt; such that Next(w, s)</t>
+  </si>
+  <si>
+    <t>Select &lt;w, a&gt; such that Next(w, a)</t>
+  </si>
+  <si>
+    <t>Select &lt;s, f&gt; such that Next(s, f)</t>
+  </si>
+  <si>
+    <t>Select &lt;s, pl&gt; such that Next(s, pl)</t>
+  </si>
+  <si>
+    <t>Select &lt;s, cl&gt; such that Next(s, cl)</t>
+  </si>
+  <si>
+    <t>Select &lt;a, f&gt; such that Next(a, f)</t>
+  </si>
+  <si>
+    <t>Select &lt;a, cl&gt; such that Next(a, cl)</t>
+  </si>
+  <si>
+    <t>Select &lt;w, f&gt; such that Next(w, f)</t>
+  </si>
+  <si>
+    <t>Select &lt;w, cl&gt; such that Next(w, cl)</t>
+  </si>
+  <si>
+    <t>Select &lt;f1, f2&gt; such that Next(f1, f2)</t>
+  </si>
+  <si>
+    <t>Select &lt;f, s&gt; such that Next(f, s)</t>
+  </si>
+  <si>
+    <t>Select &lt;f, a&gt; such that Next(f, a)</t>
+  </si>
+  <si>
+    <t>Select &lt;f, w&gt; such that Next(f, w)</t>
+  </si>
+  <si>
+    <t>Select &lt;f, cl&gt; such that Next(f, cl)</t>
+  </si>
+  <si>
+    <t>Select &lt;cl1, cl2&gt; such that Next(cl1, cl2)</t>
+  </si>
+  <si>
+    <t>Stmt While</t>
+  </si>
+  <si>
+    <t>Stmt If</t>
+  </si>
+  <si>
+    <t>Stmt Prog_Line</t>
+  </si>
+  <si>
+    <t>Stmt Call</t>
+  </si>
+  <si>
+    <t>Assign While</t>
+  </si>
+  <si>
+    <t>Assign If</t>
+  </si>
+  <si>
+    <t>Assign Call</t>
+  </si>
+  <si>
+    <t>While Stmt</t>
+  </si>
+  <si>
+    <t>While Assign</t>
+  </si>
+  <si>
+    <t>While If</t>
+  </si>
+  <si>
+    <t>While Call</t>
+  </si>
+  <si>
+    <t>If Stmt</t>
+  </si>
+  <si>
+    <t>If Assign</t>
+  </si>
+  <si>
+    <t>If While</t>
+  </si>
+  <si>
+    <t>If Call</t>
+  </si>
+  <si>
+    <t>Call Stmt</t>
+  </si>
+  <si>
+    <t>Call Assign</t>
+  </si>
+  <si>
+    <t>Call While</t>
+  </si>
+  <si>
+    <t>Call If</t>
+  </si>
+  <si>
+    <t>1 2,10 11,10 13,100 101,101 102,102 103,103 104,104 105,105 106,105 107,106 105,107 108,108 109,108 110,109 111,11 12,110 111,12 10,13 14,15 16,15 17,16 15,17 18,18 19,18 20,19 21,2 3,20 21,21 22,23 24,25 26,25 28,26 27,27 29,28 29,3 4,30 31,31 32,31 33,32 31,34 35,35 36,35 37,36 38,37 38,39 40,4 5,40 41,43 44,44 45,44 46,47 48,48 49,48 50,49 54,50 51,51 52,52 53,53 54,54 55,55 56,56 55,57 58,58 59,59 60,6 7,60 61,62 63,63 64,64 65,64 66,67 68,67 75,68 69,69 70,7 8,70 71,71 72,72 73,73 74,75 76,77 78,78 79,79 80,8 9,80 79,81 82,82 83,83 84,83 88,84 85,84 86,85 87,86 87,87 83,88 89,88 90,89 88,90 91,90 92,91 93,92 93,93 94,93 95,94 93,95 96,96 95,97 98,98 99,99 100</t>
+  </si>
+  <si>
+    <t>1 2,10 13,100 101,101 102,102 103,103 104,105 106,105 107,108 109,108 110,109 111,11 12,110 111,15 16,18 19,18 20,2 3,23 24,25 26,27 29,28 29,3 4,31 32,35 36,35 37,40 41,44 45,48 49,48 50,50 51,51 52,52 53,55 56,57 58,58 59,59 60,60 61,64 65,64 66,67 75,68 69,70 71,71 72,72 73,73 74,75 76,79 80,81 82,84 85,84 86,88 89,90 91,90 92,93 94,95 96,97 98,98 99,99 100</t>
+  </si>
+  <si>
+    <t>104 105,106 105,12 10,16 15,30 31,32 31,54 55,56 55,78 79,80 79,82 83,83 88,87 83,89 88,91 93,92 93,93 95,94 93,96 95</t>
+  </si>
+  <si>
+    <t>107 108,17 18,34 35,43 44,47 48,63 64,83 84,88 90</t>
+  </si>
+  <si>
+    <t>10 11,13 14,15 17,19 21,20 21,21 22,25 28,26 27,31 33,36 38,37 38,39 40,4 5,44 46,49 54,53 54,6 7,62 63,67 68,69 70,7 8,77 78,8 9,85 87,86 87</t>
+  </si>
+  <si>
+    <t>Select &lt;a1, a2&gt; such that Next(a1, a2)</t>
+  </si>
+  <si>
+    <t>1 2,100 101,101 102,102 103,103 104,104 105,106 105,107 108,109 111,110 111,12 10,13 14,16 15,19 21,2 3,20 21,26 27,3 4,32 31,36 38,37 38,39 40,4 5,43 44,49 54,50 51,51 52,52 53,53 54,56 55,57 58,58 59,59 60,60 61,62 63,69 70,71 72,72 73,73 74,75 76,77 78,80 79,81 82,82 83,85 87,86 87,89 88,91 93,92 93,94 93,96 95,97 98,98 99,99 100</t>
+  </si>
+  <si>
+    <t>104 105,106 105,12 10,16 15,32 31,56 55,80 79,82 83,89 88,91 93,92 93,94 93,96 95</t>
+  </si>
+  <si>
+    <t>107 108,43 44</t>
+  </si>
+  <si>
+    <t>13 14,19 21,20 21,26 27,36 38,37 38,39 40,4 5,49 54,53 54,62 63,69 70,77 78,85 87,86 87</t>
+  </si>
+  <si>
+    <t>Select &lt;w1, w2&gt; such that Next(w1, w2)</t>
+  </si>
+  <si>
+    <t>10 11,10 13,105 106,105 107,15 16,15 17,31 32,31 33,55 56,79 80,83 84,83 88,88 89,88 90,93 94,93 95,95 96</t>
+  </si>
+  <si>
+    <t>10 13,105 106,105 107,15 16,31 32,55 56,79 80,88 89,93 94,95 96</t>
+  </si>
+  <si>
+    <t>83 84,88 90</t>
+  </si>
+  <si>
+    <t>10 11,15 17,31 33</t>
+  </si>
+  <si>
+    <t>108 109,108 110,18 19,18 20,25 26,25 28,35 36,35 37,44 45,44 46,48 49,48 50,64 65,64 66,67 68,67 75,84 85,84 86,90 91,90 92</t>
+  </si>
+  <si>
+    <t>108 109,108 110,18 19,18 20,25 26,35 36,35 37,44 45,48 49,48 50,64 65,64 66,67 75,84 85,84 86,90 91,90 92</t>
+  </si>
+  <si>
+    <t>25 28,44 46,67 68</t>
+  </si>
+  <si>
+    <t>21 22,6 7,7 8,8 9</t>
+  </si>
+  <si>
+    <t>Select &lt;cl, s&gt; such that Next(cl, s)</t>
+  </si>
+  <si>
+    <t>Select &lt;cl, a&gt; such that Next(cl, a)</t>
+  </si>
+  <si>
+    <t>Select &lt;cl, w&gt; such that Next(cl, w)</t>
+  </si>
+  <si>
+    <t>Select &lt;cl, f&gt; such that Next(cl, f)</t>
+  </si>
+  <si>
+    <t>While While</t>
+  </si>
+  <si>
+    <t>If If</t>
+  </si>
+  <si>
+    <t>Call Call</t>
+  </si>
+  <si>
+    <t>1 2,100 101,101 102,102 103,103 104,109 111,110 111,2 3,3 4,50 51,51 52,52 53,57 58,58 59,59 60,60 61,71 72,72 73,73 74,75 76,81 82,97 98,98 99,99 100</t>
+  </si>
+  <si>
+    <t>83 88,93 95</t>
+  </si>
+  <si>
+    <t>11 12,17 18,21 22,23 24,27 29,28 29,30 31,34 35,40 41,47 48,54 55,6 7,63 64,68 69,7 8,70 71,78 79,8 9,87 83</t>
+  </si>
+  <si>
+    <t>11 12,23 24,27 29,28 29,40 41,68 69,70 71</t>
+  </si>
+  <si>
+    <t>30 31,54 55,78 79,87 83</t>
+  </si>
+  <si>
+    <t>17 18,34 35,47 48,63 64</t>
   </si>
 </sst>
 </file>
@@ -1799,18 +2084,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3F969A-AF06-4B88-BDEC-BD9AE21F1F8A}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD130"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="55.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="40.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="19" style="4" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="87.5703125" style="4" customWidth="1"/>
     <col min="6" max="6" width="47.28515625" style="4" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
@@ -1838,6 +2123,448 @@
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -1858,7 +2585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718E38E7-CAC6-4E2F-9E82-065AD53A2199}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add test for nextstar
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test9_InterProcedural/ExcelQuery.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test9_InterProcedural/ExcelQuery.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uses" sheetId="15" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="515">
   <si>
     <t>Index</t>
   </si>
@@ -1418,6 +1418,159 @@
   </si>
   <si>
     <t>17 18,34 35,47 48,63 64</t>
+  </si>
+  <si>
+    <t>Select &lt;s1, s2&gt; such that Next*(s1, s2)</t>
+  </si>
+  <si>
+    <t>Select &lt;s, a&gt; such that Next*(s, a)</t>
+  </si>
+  <si>
+    <t>Select &lt;s, w&gt; such that Next*(s, w)</t>
+  </si>
+  <si>
+    <t>Select &lt;s, f&gt; such that Next*(s, f)</t>
+  </si>
+  <si>
+    <t>Select &lt;s, pl&gt; such that Next*(s, pl)</t>
+  </si>
+  <si>
+    <t>Select &lt;s, cl&gt; such that Next*(s, cl)</t>
+  </si>
+  <si>
+    <t>Select &lt;a1, a2&gt; such that Next*(a1, a2)</t>
+  </si>
+  <si>
+    <t>Select &lt;a, s&gt; such that Next*(a, s)</t>
+  </si>
+  <si>
+    <t>Select &lt;a, w&gt; such that Next*(a, w)</t>
+  </si>
+  <si>
+    <t>Select &lt;a, f&gt; such that Next*(a, f)</t>
+  </si>
+  <si>
+    <t>Select &lt;a, cl&gt; such that Next*(a, cl)</t>
+  </si>
+  <si>
+    <t>Select &lt;w1, w2&gt; such that Next*(w1, w2)</t>
+  </si>
+  <si>
+    <t>Select &lt;w, s&gt; such that Next*(w, s)</t>
+  </si>
+  <si>
+    <t>Select &lt;w, a&gt; such that Next*(w, a)</t>
+  </si>
+  <si>
+    <t>Select &lt;w, f&gt; such that Next*(w, f)</t>
+  </si>
+  <si>
+    <t>Select &lt;w, cl&gt; such that Next*(w, cl)</t>
+  </si>
+  <si>
+    <t>Select &lt;f1, f2&gt; such that Next*(f1, f2)</t>
+  </si>
+  <si>
+    <t>Select &lt;f, s&gt; such that Next*(f, s)</t>
+  </si>
+  <si>
+    <t>Select &lt;f, a&gt; such that Next*(f, a)</t>
+  </si>
+  <si>
+    <t>Select &lt;f, w&gt; such that Next*(f, w)</t>
+  </si>
+  <si>
+    <t>Select &lt;f, cl&gt; such that Next*(f, cl)</t>
+  </si>
+  <si>
+    <t>Select &lt;cl1, cl2&gt; such that Next*(cl1, cl2)</t>
+  </si>
+  <si>
+    <t>Select &lt;cl, s&gt; such that Next*(cl, s)</t>
+  </si>
+  <si>
+    <t>Select &lt;cl, a&gt; such that Next*(cl, a)</t>
+  </si>
+  <si>
+    <t>Select &lt;cl, w&gt; such that Next*(cl, w)</t>
+  </si>
+  <si>
+    <t>Select &lt;cl, f&gt; such that Next*(cl, f)</t>
+  </si>
+  <si>
+    <t>1 2,1 3,1 4,1 5,10 10,10 11,10 12,10 13,10 14,100 101,100 102,100 103,100 104,100 105,100 106,100 107,100 108,100 109,100 110,100 111,101 102,101 103,101 104,101 105,101 106,101 107,101 108,101 109,101 110,101 111,102 103,102 104,102 105,102 106,102 107,102 108,102 109,102 110,102 111,103 104,103 105,103 106,103 107,103 108,103 109,103 110,103 111,104 105,104 106,104 107,104 108,104 109,104 110,104 111,105 105,105 106,105 107,105 108,105 109,105 110,105 111,106 105,106 106,106 107,106 108,106 109,106 110,106 111,107 108,107 109,107 110,107 111,108 109,108 110,108 111,109 111,11 10,11 11,11 12,11 13,11 14,110 111,12 10,12 11,12 12,12 13,12 14,13 14,15 15,15 16,15 17,15 18,15 19,15 20,15 21,15 22,16 15,16 16,16 17,16 18,16 19,16 20,16 21,16 22,17 18,17 19,17 20,17 21,17 22,18 19,18 20,18 21,18 22,19 21,19 22,2 3,2 4,2 5,20 21,20 22,21 22,23 24,25 26,25 27,25 28,25 29,26 27,26 29,27 29,28 29,3 4,3 5,30 31,30 32,30 33,31 31,31 32,31 33,32 31,32 32,32 33,34 35,34 36,34 37,34 38,35 36,35 37,35 38,36 38,37 38,39 40,39 41,4 5,40 41,43 44,43 45,43 46,44 45,44 46,47 48,47 49,47 50,47 51,47 52,47 53,47 54,47 55,47 56,48 49,48 50,48 51,48 52,48 53,48 54,48 55,48 56,49 54,49 55,49 56,50 51,50 52,50 53,50 54,50 55,50 56,51 52,51 53,51 54,51 55,51 56,52 53,52 54,52 55,52 56,53 54,53 55,53 56,54 55,54 56,55 55,55 56,56 55,56 56,57 58,57 59,57 60,57 61,58 59,58 60,58 61,59 60,59 61,6 7,6 8,6 9,60 61,62 63,62 64,62 65,62 66,63 64,63 65,63 66,64 65,64 66,67 68,67 69,67 70,67 71,67 72,67 73,67 74,67 75,67 76,68 69,68 70,68 71,68 72,68 73,68 74,69 70,69 71,69 72,69 73,69 74,7 8,7 9,70 71,70 72,70 73,70 74,71 72,71 73,71 74,72 73,72 74,73 74,75 76,77 78,77 79,77 80,78 79,78 80,79 79,79 80,8 9,80 79,80 80,81 82,81 83,81 84,81 85,81 86,81 87,81 88,81 89,81 90,81 91,81 92,81 93,81 94,81 95,81 96,82 83,82 84,82 85,82 86,82 87,82 88,82 89,82 90,82 91,82 92,82 93,82 94,82 95,82 96,83 83,83 84,83 85,83 86,83 87,83 88,83 89,83 90,83 91,83 92,83 93,83 94,83 95,83 96,84 83,84 84,84 85,84 86,84 87,84 88,84 89,84 90,84 91,84 92,84 93,84 94,84 95,84 96,85 83,85 84,85 85,85 86,85 87,85 88,85 89,85 90,85 91,85 92,85 93,85 94,85 95,85 96,86 83,86 84,86 85,86 86,86 87,86 88,86 89,86 90,86 91,86 92,86 93,86 94,86 95,86 96,87 83,87 84,87 85,87 86,87 87,87 88,87 89,87 90,87 91,87 92,87 93,87 94,87 95,87 96,88 88,88 89,88 90,88 91,88 92,88 93,88 94,88 95,88 96,89 88,89 89,89 90,89 91,89 92,89 93,89 94,89 95,89 96,90 91,90 92,90 93,90 94,90 95,90 96,91 93,91 94,91 95,91 96,92 93,92 94,92 95,92 96,93 93,93 94,93 95,93 96,94 93,94 94,94 95,94 96,95 95,95 96,96 95,96 96,97 100,97 101,97 102,97 103,97 104,97 105,97 106,97 107,97 108,97 109,97 110,97 111,97 98,97 99,98 100,98 101,98 102,98 103,98 104,98 105,98 106,98 107,98 108,98 109,98 110,98 111,98 99,99 100,99 101,99 102,99 103,99 104,99 105,99 106,99 107,99 108,99 109,99 110,99 111</t>
+  </si>
+  <si>
+    <t>10 10,100 105,101 105,102 105,103 105,104 105,105 105,106 105,11 10,12 10,15 15,16 15,30 31,31 31,32 31,47 55,48 55,49 55,50 55,51 55,52 55,53 55,54 55,55 55,56 55,77 79,78 79,79 79,80 79,81 83,81 88,81 93,81 95,82 83,82 88,82 93,82 95,83 83,83 88,83 93,83 95,84 83,84 88,84 93,84 95,85 83,85 88,85 93,85 95,86 83,86 88,86 93,86 95,87 83,87 88,87 93,87 95,88 88,88 93,88 95,89 88,89 93,89 95,90 93,90 95,91 93,91 95,92 93,92 95,93 93,93 95,94 93,94 95,95 95,96 95,97 105,98 105,99 105</t>
+  </si>
+  <si>
+    <t>1 2,1 3,1 4,10 12,10 13,100 101,100 102,100 103,100 104,100 106,100 107,100 109,100 110,100 111,101 102,101 103,101 104,101 106,101 107,101 109,101 110,101 111,102 103,102 104,102 106,102 107,102 109,102 110,102 111,103 104,103 106,103 107,103 109,103 110,103 111,104 106,104 107,104 109,104 110,104 111,105 106,105 107,105 109,105 110,105 111,106 106,106 107,106 109,106 110,106 111,107 109,107 110,107 111,108 109,108 110,108 111,109 111,11 12,11 13,110 111,12 12,12 13,15 16,15 19,15 20,16 16,16 19,16 20,17 19,17 20,18 19,18 20,2 3,2 4,23 24,25 26,25 29,26 29,27 29,28 29,3 4,30 32,31 32,32 32,34 36,34 37,35 36,35 37,39 41,40 41,43 45,44 45,47 49,47 50,47 51,47 52,47 53,47 56,48 49,48 50,48 51,48 52,48 53,48 56,49 56,50 51,50 52,50 53,50 56,51 52,51 53,51 56,52 53,52 56,53 56,54 56,55 56,56 56,57 58,57 59,57 60,57 61,58 59,58 60,58 61,59 60,59 61,60 61,62 65,62 66,63 65,63 66,64 65,64 66,67 69,67 71,67 72,67 73,67 74,67 75,67 76,68 69,68 71,68 72,68 73,68 74,69 71,69 72,69 73,69 74,70 71,70 72,70 73,70 74,71 72,71 73,71 74,72 73,72 74,73 74,75 76,77 80,78 80,79 80,80 80,81 82,81 85,81 86,81 89,81 91,81 92,81 94,81 96,82 85,82 86,82 89,82 91,82 92,82 94,82 96,83 85,83 86,83 89,83 91,83 92,83 94,83 96,84 85,84 86,84 89,84 91,84 92,84 94,84 96,85 85,85 86,85 89,85 91,85 92,85 94,85 96,86 85,86 86,86 89,86 91,86 92,86 94,86 96,87 85,87 86,87 89,87 91,87 92,87 94,87 96,88 89,88 91,88 92,88 94,88 96,89 89,89 91,89 92,89 94,89 96,90 91,90 92,90 94,90 96,91 94,91 96,92 94,92 96,93 94,93 96,94 94,94 96,95 96,96 96,97 100,97 101,97 102,97 103,97 104,97 106,97 107,97 109,97 110,97 111,97 98,97 99,98 100,98 101,98 102,98 103,98 104,98 106,98 107,98 109,98 110,98 111,98 99,99 100,99 101,99 102,99 103,99 104,99 106,99 107,99 109,99 110,99 111</t>
+  </si>
+  <si>
+    <t>100 108,101 108,102 108,103 108,104 108,105 108,106 108,107 108,15 18,16 18,17 18,34 35,43 44,47 48,62 64,63 64,81 84,81 90,82 84,82 90,83 84,83 90,84 84,84 90,85 84,85 90,86 84,86 90,87 84,87 90,88 90,89 90,97 108,98 108,99 108</t>
+  </si>
+  <si>
+    <t>1 5,10 11,10 14,11 11,11 14,12 11,12 14,13 14,15 17,15 21,15 22,16 17,16 21,16 22,17 21,17 22,18 21,18 22,19 21,19 22,2 5,20 21,20 22,21 22,25 27,25 28,26 27,3 5,30 33,31 33,32 33,34 38,35 38,36 38,37 38,39 40,4 5,43 46,44 46,47 54,48 54,49 54,50 54,51 54,52 54,53 54,6 7,6 8,6 9,62 63,67 68,67 70,68 70,69 70,7 8,7 9,77 78,8 9,81 87,82 87,83 87,84 87,85 87,86 87,87 87</t>
+  </si>
+  <si>
+    <t>1 2,1 3,1 4,100 101,100 102,100 103,100 104,100 106,100 107,100 109,100 110,100 111,101 102,101 103,101 104,101 106,101 107,101 109,101 110,101 111,102 103,102 104,102 106,102 107,102 109,102 110,102 111,103 104,103 106,103 107,103 109,103 110,103 111,104 106,104 107,104 109,104 110,104 111,106 106,106 107,106 109,106 110,106 111,107 109,107 110,107 111,109 111,110 111,12 12,12 13,16 16,16 19,16 20,2 3,2 4,26 29,3 4,32 32,39 41,43 45,49 56,50 51,50 52,50 53,50 56,51 52,51 53,51 56,52 53,52 56,53 56,56 56,57 58,57 59,57 60,57 61,58 59,58 60,58 61,59 60,59 61,60 61,62 65,62 66,69 71,69 72,69 73,69 74,71 72,71 73,71 74,72 73,72 74,73 74,75 76,77 80,80 80,81 82,81 85,81 86,81 89,81 91,81 92,81 94,81 96,82 85,82 86,82 89,82 91,82 92,82 94,82 96,85 85,85 86,85 89,85 91,85 92,85 94,85 96,86 85,86 86,86 89,86 91,86 92,86 94,86 96,89 89,89 91,89 92,89 94,89 96,91 94,91 96,92 94,92 96,94 94,94 96,96 96,97 100,97 101,97 102,97 103,97 104,97 106,97 107,97 109,97 110,97 111,97 98,97 99,98 100,98 101,98 102,98 103,98 104,98 106,98 107,98 109,98 110,98 111,98 99,99 100,99 101,99 102,99 103,99 104,99 106,99 107,99 109,99 110,99 111</t>
+  </si>
+  <si>
+    <t>1 2,1 3,1 4,1 5,100 101,100 102,100 103,100 104,100 105,100 106,100 107,100 108,100 109,100 110,100 111,101 102,101 103,101 104,101 105,101 106,101 107,101 108,101 109,101 110,101 111,102 103,102 104,102 105,102 106,102 107,102 108,102 109,102 110,102 111,103 104,103 105,103 106,103 107,103 108,103 109,103 110,103 111,104 105,104 106,104 107,104 108,104 109,104 110,104 111,106 105,106 106,106 107,106 108,106 109,106 110,106 111,107 108,107 109,107 110,107 111,109 111,110 111,12 10,12 11,12 12,12 13,12 14,13 14,16 15,16 16,16 17,16 18,16 19,16 20,16 21,16 22,19 21,19 22,2 3,2 4,2 5,20 21,20 22,26 27,26 29,3 4,3 5,32 31,32 32,32 33,36 38,37 38,39 40,39 41,4 5,43 44,43 45,43 46,49 54,49 55,49 56,50 51,50 52,50 53,50 54,50 55,50 56,51 52,51 53,51 54,51 55,51 56,52 53,52 54,52 55,52 56,53 54,53 55,53 56,56 55,56 56,57 58,57 59,57 60,57 61,58 59,58 60,58 61,59 60,59 61,60 61,62 63,62 64,62 65,62 66,69 70,69 71,69 72,69 73,69 74,71 72,71 73,71 74,72 73,72 74,73 74,75 76,77 78,77 79,77 80,80 79,80 80,81 82,81 83,81 84,81 85,81 86,81 87,81 88,81 89,81 90,81 91,81 92,81 93,81 94,81 95,81 96,82 83,82 84,82 85,82 86,82 87,82 88,82 89,82 90,82 91,82 92,82 93,82 94,82 95,82 96,85 83,85 84,85 85,85 86,85 87,85 88,85 89,85 90,85 91,85 92,85 93,85 94,85 95,85 96,86 83,86 84,86 85,86 86,86 87,86 88,86 89,86 90,86 91,86 92,86 93,86 94,86 95,86 96,89 88,89 89,89 90,89 91,89 92,89 93,89 94,89 95,89 96,91 93,91 94,91 95,91 96,92 93,92 94,92 95,92 96,94 93,94 94,94 95,94 96,96 95,96 96,97 100,97 101,97 102,97 103,97 104,97 105,97 106,97 107,97 108,97 109,97 110,97 111,97 98,97 99,98 100,98 101,98 102,98 103,98 104,98 105,98 106,98 107,98 108,98 109,98 110,98 111,98 99,99 100,99 101,99 102,99 103,99 104,99 105,99 106,99 107,99 108,99 109,99 110,99 111</t>
+  </si>
+  <si>
+    <t>100 105,101 105,102 105,103 105,104 105,106 105,12 10,16 15,32 31,49 55,50 55,51 55,52 55,53 55,56 55,77 79,80 79,81 83,81 88,81 93,81 95,82 83,82 88,82 93,82 95,85 83,85 88,85 93,85 95,86 83,86 88,86 93,86 95,89 88,89 93,89 95,91 93,91 95,92 93,92 95,94 93,94 95,96 95,97 105,98 105,99 105</t>
+  </si>
+  <si>
+    <t>100 108,101 108,102 108,103 108,104 108,106 108,107 108,16 18,43 44,62 64,81 84,81 90,82 84,82 90,85 84,85 90,86 84,86 90,89 90,97 108,98 108,99 108</t>
+  </si>
+  <si>
+    <t>1 5,12 11,12 14,13 14,16 17,16 21,16 22,19 21,19 22,2 5,20 21,20 22,26 27,3 5,32 33,36 38,37 38,39 40,4 5,43 46,49 54,50 54,51 54,52 54,53 54,62 63,69 70,77 78,81 87,82 87,85 87,86 87</t>
+  </si>
+  <si>
+    <t>10 10,105 105,15 15,31 31,55 55,79 79,83 83,83 88,83 93,83 95,88 88,88 93,88 95,93 93,93 95,95 95</t>
+  </si>
+  <si>
+    <t>10 10,10 11,10 12,10 13,10 14,105 105,105 106,105 107,105 108,105 109,105 110,105 111,15 15,15 16,15 17,15 18,15 19,15 20,15 21,15 22,31 31,31 32,31 33,55 55,55 56,79 79,79 80,83 83,83 84,83 85,83 86,83 87,83 88,83 89,83 90,83 91,83 92,83 93,83 94,83 95,83 96,88 88,88 89,88 90,88 91,88 92,88 93,88 94,88 95,88 96,93 93,93 94,93 95,93 96,95 95,95 96</t>
+  </si>
+  <si>
+    <t>10 12,10 13,105 106,105 107,105 109,105 110,105 111,15 16,15 19,15 20,31 32,55 56,79 80,83 85,83 86,83 89,83 91,83 92,83 94,83 96,88 89,88 91,88 92,88 94,88 96,93 94,93 96,95 96</t>
+  </si>
+  <si>
+    <t>105 108,15 18,83 84,83 90,88 90</t>
+  </si>
+  <si>
+    <t>10 11,10 14,15 17,15 21,15 22,31 33,83 87</t>
+  </si>
+  <si>
+    <t>84 84,84 90</t>
+  </si>
+  <si>
+    <t>108 109,108 110,108 111,18 19,18 20,18 21,18 22,25 26,25 27,25 28,25 29,35 36,35 37,35 38,44 45,44 46,48 49,48 50,48 51,48 52,48 53,48 54,48 55,48 56,64 65,64 66,67 68,67 69,67 70,67 71,67 72,67 73,67 74,67 75,67 76,84 83,84 84,84 85,84 86,84 87,84 88,84 89,84 90,84 91,84 92,84 93,84 94,84 95,84 96,90 91,90 92,90 93,90 94,90 95,90 96</t>
+  </si>
+  <si>
+    <t>108 109,108 110,108 111,18 19,18 20,25 26,25 29,35 36,35 37,44 45,48 49,48 50,48 51,48 52,48 53,48 56,64 65,64 66,67 69,67 71,67 72,67 73,67 74,67 75,67 76,84 85,84 86,84 89,84 91,84 92,84 94,84 96,90 91,90 92,90 94,90 96</t>
+  </si>
+  <si>
+    <t>48 55,84 83,84 88,84 93,84 95,90 93,90 95</t>
+  </si>
+  <si>
+    <t>18 21,18 22,25 27,25 28,35 38,44 46,48 54,67 68,67 70,84 87</t>
+  </si>
+  <si>
+    <t>11 11,11 14,17 21,17 22,21 22,30 33,34 38,47 54,6 7,6 8,6 9,68 70,7 8,7 9,8 9,87 87</t>
+  </si>
+  <si>
+    <t>11 10,11 11,11 12,11 13,11 14,17 18,17 19,17 20,17 21,17 22,21 22,23 24,27 29,28 29,30 31,30 32,30 33,34 35,34 36,34 37,34 38,40 41,47 48,47 49,47 50,47 51,47 52,47 53,47 54,47 55,47 56,54 55,54 56,6 7,6 8,6 9,63 64,63 65,63 66,68 69,68 70,68 71,68 72,68 73,68 74,7 8,7 9,70 71,70 72,70 73,70 74,78 79,78 80,8 9,87 83,87 84,87 85,87 86,87 87,87 88,87 89,87 90,87 91,87 92,87 93,87 94,87 95,87 96</t>
+  </si>
+  <si>
+    <t>11 12,11 13,17 19,17 20,23 24,27 29,28 29,30 32,34 36,34 37,40 41,47 49,47 50,47 51,47 52,47 53,47 56,54 56,63 65,63 66,68 69,68 71,68 72,68 73,68 74,70 71,70 72,70 73,70 74,78 80,87 85,87 86,87 89,87 91,87 92,87 94,87 96</t>
+  </si>
+  <si>
+    <t>11 10,30 31,47 55,54 55,78 79,87 83,87 88,87 93,87 95</t>
+  </si>
+  <si>
+    <t>17 18,34 35,47 48,63 64,87 84,87 90</t>
   </si>
 </sst>
 </file>
@@ -1519,7 +1672,31 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF57BB8A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE67C73"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2013,10 +2190,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"BUG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2027,66 +2204,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52217274-FA67-4C83-B4A0-40B0A8F765E5}">
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD133"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="43.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="40.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="87.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="47.28515625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
-      <formula>"BUG"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
-      <formula>"PASS"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3F969A-AF06-4B88-BDEC-BD9AE21F1F8A}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -2133,10 +2253,10 @@
         <v>369</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>370</v>
+        <v>464</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>432</v>
+        <v>490</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>104</v>
@@ -2150,10 +2270,10 @@
         <v>105</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>394</v>
+        <v>465</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>433</v>
+        <v>492</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>107</v>
@@ -2167,10 +2287,10 @@
         <v>371</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>395</v>
+        <v>466</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>434</v>
+        <v>491</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>413</v>
@@ -2184,10 +2304,10 @@
         <v>372</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>400</v>
+        <v>467</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>435</v>
+        <v>493</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>414</v>
@@ -2201,10 +2321,10 @@
         <v>373</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>401</v>
+        <v>468</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>432</v>
+        <v>490</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>415</v>
@@ -2218,10 +2338,10 @@
         <v>374</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>402</v>
+        <v>469</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>436</v>
+        <v>494</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>416</v>
@@ -2235,10 +2355,10 @@
         <v>111</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>437</v>
+        <v>470</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>458</v>
+        <v>495</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>110</v>
@@ -2252,10 +2372,10 @@
         <v>375</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>396</v>
+        <v>471</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>438</v>
+        <v>496</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>109</v>
@@ -2269,10 +2389,10 @@
         <v>376</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>397</v>
+        <v>472</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>439</v>
+        <v>497</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>417</v>
@@ -2286,10 +2406,10 @@
         <v>377</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>403</v>
+        <v>473</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>440</v>
+        <v>498</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>418</v>
@@ -2303,10 +2423,10 @@
         <v>378</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>404</v>
+        <v>474</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>441</v>
+        <v>499</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>419</v>
@@ -2320,10 +2440,10 @@
         <v>379</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>442</v>
+        <v>475</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>459</v>
+        <v>500</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>455</v>
@@ -2337,10 +2457,10 @@
         <v>380</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>398</v>
+        <v>476</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>443</v>
+        <v>501</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>420</v>
@@ -2354,10 +2474,10 @@
         <v>381</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>399</v>
+        <v>477</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>444</v>
+        <v>502</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>421</v>
@@ -2371,10 +2491,10 @@
         <v>382</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>405</v>
+        <v>478</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>445</v>
+        <v>503</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>422</v>
@@ -2388,10 +2508,10 @@
         <v>383</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>406</v>
+        <v>479</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>446</v>
+        <v>504</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>423</v>
@@ -2405,10 +2525,10 @@
         <v>384</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>407</v>
+        <v>480</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>73</v>
+        <v>505</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>456</v>
@@ -2422,10 +2542,10 @@
         <v>385</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>408</v>
+        <v>481</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>447</v>
+        <v>506</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>424</v>
@@ -2439,10 +2559,10 @@
         <v>386</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>409</v>
+        <v>482</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>448</v>
+        <v>507</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>425</v>
@@ -2456,10 +2576,10 @@
         <v>387</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>410</v>
+        <v>483</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>73</v>
+        <v>508</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>426</v>
@@ -2473,10 +2593,10 @@
         <v>388</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>411</v>
+        <v>484</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>449</v>
+        <v>509</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>427</v>
@@ -2490,10 +2610,10 @@
         <v>389</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>412</v>
+        <v>485</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>450</v>
+        <v>510</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>457</v>
@@ -2507,10 +2627,10 @@
         <v>390</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>451</v>
+        <v>486</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>460</v>
+        <v>511</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>428</v>
@@ -2524,10 +2644,10 @@
         <v>391</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>452</v>
+        <v>487</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>461</v>
+        <v>512</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>429</v>
@@ -2541,10 +2661,10 @@
         <v>392</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>453</v>
+        <v>488</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>462</v>
+        <v>513</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>430</v>
@@ -2558,6 +2678,505 @@
         <v>393</v>
       </c>
       <c r="C27" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>431</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"BUG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3F969A-AF06-4B88-BDEC-BD9AE21F1F8A}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="4" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="87.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="47.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>437</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>397</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>442</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>399</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>408</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>411</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>453</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>454</v>
       </c>
       <c r="D27" s="5" t="s">
@@ -2569,10 +3188,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>"BUG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3437,10 +4056,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G2">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"BUG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4075,10 +4694,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G2">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"BUG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5184,10 +5803,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"BUG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6274,10 +6893,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"BUG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>